<commit_message>
Update to final publication zib MedicalDevice
</commit_message>
<xml_diff>
--- a/maps/xtehr2zibs2024/Device-and-DeviceUse-full.xlsx
+++ b/maps/xtehr2zibs2024/Device-and-DeviceUse-full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,60 +456,70 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>alias_zib</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>type_zib</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>card._zib</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>stereotype_zib</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>id_zib</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>definition_zib</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>definitioncode_zib</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>id_xtehr</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>path_xtehr</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>short_xtehr</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>definition_xtehr</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>type_xtehr</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>card._xtehr</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>binding_xtehr</t>
         </is>
@@ -536,54 +546,64 @@
           <t>MedicalDevice.Product</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NL: Product</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>container</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>NL-CM:10.1.2</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>The medical device (internally or externally).</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>405815000 Procedure device</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>SNOMED CT: 405815000 Procedure device</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>EHDSDevice</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>EHDSDevice</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>Device model</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>C.12 - EHDS refined base model for Device information</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>0..*</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -599,37 +619,39 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr">
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
         <is>
           <t>EHDSDevice.expiryDate</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>EHDSDevice.expiryDate</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>C.12.4 - Expiry date</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>The date and time beyond which this device is no longer valid or should not be used (if applicable).</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>dateTime</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -654,57 +676,67 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>NL: ProductID</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>ST</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>NL-CM:10.1.16</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Globally unique identification of the product, for example the serial number or a UDI (unique device identifier). For some products, the law requires the use of a UDI. Commonly used coding systems are HIBC and GS1/GTIN.
 A UDI often contains more information than just an ID, but also, for example, an expiration date. If a UDI is used, the entire code can be included as text in ProductID, so that no important information is lost.</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
         <is>
           <t>EHDSDevice.identifier</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>EHDSDevice.identifier</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>C.12.1 - Identifier</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>An identifier of the device which is unique within in a defined scope. Multiple identifiers can be used.</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>Identifier</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>1..*</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -720,37 +752,39 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
         <is>
           <t>EHDSDevice.lotNumber</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>EHDSDevice.lotNumber</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>C.12.5 - Lot number</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>Lot number of manufacture</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -766,37 +800,39 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
         <is>
           <t>EHDSDevice.manufactureDate</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>EHDSDevice.manufactureDate</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>C.12.3 - Manufacture date</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>The date and time when the device was manufactured</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>dateTime</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -812,37 +848,39 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
         <is>
           <t>EHDSDevice.manufacturer</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>EHDSDevice.manufacturer</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>C.12.2 - Manufacturer</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>Name of device manufacturer</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -858,37 +896,39 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
         <is>
           <t>EHDSDevice.modelNumber</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>EHDSDevice.modelNumber</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>C.12.8 - Model number</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>The manufacturer's model number for the device</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -904,37 +944,39 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
         <is>
           <t>EHDSDevice.name</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>EHDSDevice.name</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>C.12.7 - Name</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>The name and name type of the device as known to the manufacturer and/or patient</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>0..*</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -950,37 +992,39 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
         <is>
           <t>EHDSDevice.note</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>EHDSDevice.note</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>C.12.11 - Note</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>Device notes and comments</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>Narrative</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>0..*</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -996,37 +1040,39 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
         <is>
           <t>EHDSDevice.serialNumber</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>EHDSDevice.serialNumber</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>C.12.6 - Serial number</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>Serial number assigned by the manufacturer</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1051,56 +1097,66 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>NL: ProductType</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>CD</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>NL-CM:10.1.3</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>The code of the type of product.</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
         <is>
           <t>EHDSDevice.type</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>EHDSDevice.type</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>C.12.10 - Type</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>Device type</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>CodeableConcept</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>0..*</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>{'strength': 'preferred', 'description': 'SNOMED CT, EMDN'}</t>
         </is>
@@ -1120,37 +1176,39 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr">
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
         <is>
           <t>EHDSDevice.version</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>EHDSDevice.version</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>C.12.9 - Version</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>The actual design of the device or software version running on the device</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1173,50 +1231,60 @@
           <t>MedicalDevice</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>NL: MedischHulpmiddel</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>rootconcept</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>NL-CM:10.1.1</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Root concept of the MedicalDevice information model. This root concept contains all data elements of the MedicalDevice information model.</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>49062001 Device</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>SNOMED CT: 49062001 Device</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>EHDSDeviceUse</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>EHDSDeviceUse</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>Device use model</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>EHDS refined base model for Device Use</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr">
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>0..*</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1239,58 +1307,68 @@
           <t>MedicalDevice.AnatomicalLocation</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>NL: AnatomischeLocatie</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>data,reference</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>NL-CM:10.1.15</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Patient’s anatomical location of the medical device used.</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>363698007 Finding site</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>SNOMED CT: 363698007 Finding site</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.bodySite</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.bodySite</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>Anatomical location of the device. May include laterality.</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>Anatomical location of the device. May include laterality.</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>CodeableConcept</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1306,37 +1384,39 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.device</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.device</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>The details of the device used.</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>The details of the device used.</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>EHDSDevice</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>1..1</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1361,56 +1441,66 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>NL: EindDatum</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>TS</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>NL-CM:10.1.14</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>The end date of the last use or explant of the medical device. A ‘vague’ date, such as only the year, is permitted.</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.endDate</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.endDate</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>Date when the device was explanted from the patient or the external device was no longer in use; likewise when the device is planned to be explanted.</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="O17" t="inlineStr">
         <is>
           <t>Date when the device was explanted from the patient or the external device was no longer in use; likewise when the device is planned to be explanted.</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
+      <c r="P17" t="inlineStr">
         <is>
           <t>dateTime</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1426,37 +1516,39 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr">
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.identifier</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.identifier</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>An identifier for this statement.</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="O18" t="inlineStr">
         <is>
           <t>An identifier for this statement.</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>Identifier</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="Q18" t="inlineStr">
         <is>
           <t>0..*</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1481,56 +1573,66 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>NL: BeginDatum</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
           <t>TS</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>NL-CM:10.1.11</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>The start date of the first use or implant of the medical device. A ‘vague’ date, such as only the year, is permitted.</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.implantDate</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.implantDate</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>Date when procedure was performed.</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="O19" t="inlineStr">
         <is>
           <t>Date when procedure was performed.</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
+      <c r="P19" t="inlineStr">
         <is>
           <t>dateTime</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="Q19" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1555,60 +1657,70 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>NL: Toelichting</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>ST</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>NL-CM:10.1.10</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>Comment about use or information on the medical device used.</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>48767-8 Annotation comment [Interpretation] Narrative</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>LOINC: 48767-8 Annotation comment [Interpretation] Narrative</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.note</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>EHDSDeviceUse.note</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>Note about the device statement that were not represented at all or sufficiently in one of the attributes provided in a class. These may include for example a comment, an instruction, or a note associated with the statement.</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="O20" t="inlineStr">
         <is>
           <t>Note about the device statement that were not represented at all or sufficiently in one of the attributes provided in a class. These may include for example a comment, an instruction, or a note associated with the statement.</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="Q20" t="inlineStr">
         <is>
           <t>0..*</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1631,42 +1743,44 @@
           <t>MedicalDevice.Indication::Diagnosis</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>NL: Indicatie::Diagnose</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
         <is>
           <t>0..*</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>context,reference</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>NL-CM:10.1.17</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>The diagnosis as indication for the medical device.</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.reason</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>MedicalDevice.Indication::Problem</t>
-        </is>
-      </c>
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
@@ -1676,14 +1790,44 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>EHDSDeviceUse.reason[x]</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>EHDSDeviceUse.reason[x]</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Reason or justification for the use of the device.</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Reason or justification for the use of the device.</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>EHDSCondition</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>0..*</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>EHDSDeviceUse.recorded</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
@@ -1692,42 +1836,44 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.reason[x]</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.reason[x]</t>
-        </is>
-      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Reason or justification for the use of the device.</t>
+          <t>EHDSDeviceUse.recorded</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Reason or justification for the use of the device.</t>
+          <t>EHDSDeviceUse.recorded</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>EHDSCondition</t>
+          <t>Date and time at which the statement was made/recorded.</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>0..*</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr"/>
+          <t>Date and time at which the statement was made/recorded.</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>dateTime</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>0..1</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>EHDSDeviceUse.recorded</t>
+          <t>EHDSDeviceUse.source</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1738,44 +1884,18 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.recorded</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.recorded</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Date and time at which the statement was made/recorded.</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>Date and time at which the statement was made/recorded.</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>dateTime</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>0..1</t>
-        </is>
-      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.source</t>
-        </is>
-      </c>
+      <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
@@ -1786,14 +1906,44 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>EHDSDeviceUse.source[x]</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>EHDSDeviceUse.source[x]</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Who reported the device was being used by the patient.</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Who reported the device was being used by the patient.</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>EHDSPatient</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>0..1</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>EHDSDeviceUse.status</t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
@@ -1802,42 +1952,48 @@
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.source[x]</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.source[x]</t>
-        </is>
-      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Who reported the device was being used by the patient.</t>
+          <t>EHDSDeviceUse.status</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Who reported the device was being used by the patient.</t>
+          <t>EHDSDeviceUse.status</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>EHDSPatient</t>
+          <t>Current status of the Device Usage.</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
+          <t>Current status of the Device Usage.</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>CodeableConcept</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>{'strength': 'preferred', 'description': 'HL7 device-statement-status'}</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>EHDSDeviceUse.status</t>
+          <t>EHDSDeviceUse.subject</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1848,217 +2004,199 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.status</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.status</t>
-        </is>
-      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Current status of the Device Usage.</t>
+          <t>EHDSDeviceUse.subject</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Current status of the Device Usage.</t>
+          <t>EHDSDeviceUse.subject</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>CodeableConcept</t>
+          <t>The patient using the device.</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
+          <t>The patient using the device.</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>EHDSPatient</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>1..1</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>MedicalDevice.HealthProfessional</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>HealthProfessional</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>MedicalDevice.HealthProfessional</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>NL: Zorgverlener</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>{'strength': 'preferred', 'description': 'HL7 device-statement-status'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.subject</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>context,reference</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>NL-CM:10.1.9</t>
+        </is>
+      </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>EHDSDeviceUse.subject</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>EHDSDeviceUse.subject</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>The patient using the device.</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>The patient using the device.</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>EHDSPatient</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>1..1</t>
-        </is>
-      </c>
+          <t>The health professional involved in the indication for use of the medical device implant.</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MedicalDevice.HealthProfessional</t>
+          <t>MedicalDevice.Location::HealthcareProvider</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>HealthProfessional</t>
+          <t>Location::HealthcareProvider</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>MedicalDevice.HealthProfessional</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr">
+          <t>MedicalDevice.Location::HealthcareProvider</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>NL: Locatie::Zorgaanbieder</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
         <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>NL-CM:10.1.9</t>
-        </is>
-      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>The health professional involved in the indication for use of the medical device implant.</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
+          <t>context,reference</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>NL-CM:10.1.8</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>The healthcare provider where use of the medical device was initiated or where the aid was implanted.</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MedicalDevice.Location::HealthcareProvider</t>
+          <t>MedicalDevice.ProductDescription</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Location::HealthcareProvider</t>
+          <t>ProductDescription</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>MedicalDevice.Location::HealthcareProvider</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
+          <t>MedicalDevice.ProductDescription</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>NL: ProductOmschrijving</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>ST</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>0..1</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>NL-CM:10.1.8</t>
-        </is>
-      </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>The healthcare provider where use of the medical device was initiated or where the aid was implanted.</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>NL-CM:10.1.13</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Textual description of the product.</t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>MedicalDevice.ProductDescription</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>ProductDescription</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>MedicalDevice.ProductDescription</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>ST</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>0..1</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>NL-CM:10.1.13</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Textual description of the product.</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>